<commit_message>
Prepare final plot versions for article submission
</commit_message>
<xml_diff>
--- a/data/caver_models/CastP_volume_rawdata.xlsx
+++ b/data/caver_models/CastP_volume_rawdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robi0916/Documents/University_of_Minnesota/Wackett_Lab/github/synbio-data-analysis/data/caver_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38FC26D-ACC3-BC4D-A681-97C9D8A0B769}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA9C19E-9D8F-C94A-909F-64E20D9C47E4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-65040" yWindow="460" windowWidth="30660" windowHeight="25220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CastP_submission_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1058,13 +1059,14 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1423,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1459,122 +1461,128 @@
     </row>
     <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>170</v>
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
       </c>
       <c r="C2" s="5">
-        <v>256.959</v>
+        <v>776.39499999999998</v>
       </c>
       <c r="D2" s="5">
-        <v>69.838999999999999</v>
-      </c>
-      <c r="E2">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F2" t="s">
-        <v>128</v>
+        <v>780.87599999999998</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>172</v>
+        <v>95</v>
       </c>
       <c r="C3" s="5">
-        <v>497.26799999999997</v>
+        <v>657.00800000000004</v>
       </c>
       <c r="D3" s="5">
-        <v>230.96</v>
-      </c>
-      <c r="E3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>478.9</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4">
-        <v>598.21699999999998</v>
-      </c>
-      <c r="D4">
-        <v>446.63200000000001</v>
-      </c>
-      <c r="E4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
+        <v>151</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="5">
+        <v>613.40099999999995</v>
+      </c>
+      <c r="D4" s="5">
+        <v>457.71</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="2">
-        <v>561.40200000000004</v>
-      </c>
-      <c r="D5" s="2">
-        <v>354.00299999999999</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>128</v>
+        <v>146</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>598.21699999999998</v>
+      </c>
+      <c r="D5">
+        <v>446.63200000000001</v>
+      </c>
+      <c r="E5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>56</v>
+        <v>156</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C6" s="5">
-        <v>776.39499999999998</v>
+        <v>555.57299999999998</v>
       </c>
       <c r="D6" s="5">
-        <v>780.87599999999998</v>
+        <v>415.82400000000001</v>
       </c>
       <c r="E6" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="5">
-        <v>253.49700000000001</v>
-      </c>
-      <c r="D7" s="5">
-        <v>115.92100000000001</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="2">
+        <v>561.40200000000004</v>
+      </c>
+      <c r="D7" s="2">
+        <v>354.00299999999999</v>
       </c>
       <c r="E7" s="4">
         <v>2.2000000000000002</v>
@@ -1585,16 +1593,16 @@
     </row>
     <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C8" s="5">
-        <v>555.57299999999998</v>
+        <v>629.94399999999996</v>
       </c>
       <c r="D8" s="5">
-        <v>415.82400000000001</v>
+        <v>344.88299999999998</v>
       </c>
       <c r="E8" s="4">
         <v>2.2000000000000002</v>
@@ -1603,21 +1611,21 @@
         <v>128</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>157</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>161</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C9" s="5">
-        <v>286.87799999999999</v>
+        <v>551.10900000000004</v>
       </c>
       <c r="D9" s="5">
-        <v>184.35400000000001</v>
+        <v>344.66</v>
       </c>
       <c r="E9" s="4">
         <v>2.2000000000000002</v>
@@ -1626,21 +1634,21 @@
         <v>128</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>158</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C10" s="5">
-        <v>232.20400000000001</v>
+        <v>547.16499999999996</v>
       </c>
       <c r="D10" s="5">
-        <v>120.45099999999999</v>
+        <v>329.22199999999998</v>
       </c>
       <c r="E10" s="4">
         <v>2.2000000000000002</v>
@@ -1649,21 +1657,21 @@
         <v>128</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C11" s="5">
-        <v>451.37400000000002</v>
+        <v>500.26</v>
       </c>
       <c r="D11" s="5">
-        <v>211.19200000000001</v>
+        <v>304.78500000000003</v>
       </c>
       <c r="E11" s="4">
         <v>2.2000000000000002</v>
@@ -1674,36 +1682,39 @@
     </row>
     <row r="12" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="C12" s="5">
-        <v>425.96899999999999</v>
+        <v>519.96400000000006</v>
       </c>
       <c r="D12" s="5">
-        <v>275.464</v>
+        <v>304.73</v>
       </c>
       <c r="E12" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G12" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>42</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="C13" s="5">
-        <v>407.09100000000001</v>
+        <v>579.18700000000001</v>
       </c>
       <c r="D13" s="5">
-        <v>182.328</v>
+        <v>303.61900000000003</v>
       </c>
       <c r="E13" s="4">
         <v>2.2000000000000002</v>
@@ -1714,105 +1725,105 @@
     </row>
     <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C14" s="5">
-        <v>171.90299999999999</v>
+        <v>556.245</v>
       </c>
       <c r="D14" s="5">
-        <v>51.412999999999997</v>
+        <v>300.33699999999999</v>
       </c>
       <c r="E14" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C15" s="5">
-        <v>551.10900000000004</v>
+        <v>306.78300000000002</v>
       </c>
       <c r="D15" s="5">
-        <v>344.66</v>
+        <v>291.78500000000003</v>
       </c>
       <c r="E15" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="C16" s="5">
-        <v>500.26</v>
+        <v>511.01600000000002</v>
       </c>
       <c r="D16" s="5">
-        <v>304.78500000000003</v>
+        <v>282.154</v>
       </c>
       <c r="E16" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G16" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C17" s="5">
-        <v>306.78300000000002</v>
+        <v>537.31700000000001</v>
       </c>
       <c r="D17" s="5">
-        <v>291.78500000000003</v>
+        <v>277.05700000000002</v>
       </c>
       <c r="E17" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C18" s="5">
-        <v>260.495</v>
+        <v>425.96899999999999</v>
       </c>
       <c r="D18" s="5">
-        <v>95.259</v>
+        <v>275.464</v>
       </c>
       <c r="E18" s="4">
         <v>2.2000000000000002</v>
@@ -1823,16 +1834,16 @@
     </row>
     <row r="19" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C19" s="5">
-        <v>347.57</v>
+        <v>429.28300000000002</v>
       </c>
       <c r="D19" s="5">
-        <v>226.02</v>
+        <v>274.56200000000001</v>
       </c>
       <c r="E19" s="4">
         <v>2.2000000000000002</v>
@@ -1841,21 +1852,21 @@
         <v>128</v>
       </c>
       <c r="G19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20">
-        <v>496.00900000000001</v>
-      </c>
-      <c r="D20">
-        <v>230.708</v>
+        <v>112</v>
+      </c>
+      <c r="C20" s="5">
+        <v>547.33600000000001</v>
+      </c>
+      <c r="D20" s="5">
+        <v>267.74400000000003</v>
       </c>
       <c r="E20" s="4">
         <v>2.2000000000000002</v>
@@ -1866,36 +1877,39 @@
     </row>
     <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="C21" s="5">
-        <v>537.31700000000001</v>
+        <v>448.435</v>
       </c>
       <c r="D21" s="5">
-        <v>277.05700000000002</v>
+        <v>263.34899999999999</v>
       </c>
       <c r="E21" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G21" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="C22" s="5">
-        <v>257.899</v>
+        <v>576.09500000000003</v>
       </c>
       <c r="D22" s="5">
-        <v>135.018</v>
+        <v>257.839</v>
       </c>
       <c r="E22" s="4">
         <v>2.2000000000000002</v>
@@ -1904,21 +1918,21 @@
         <v>128</v>
       </c>
       <c r="G22" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C23" s="5">
-        <v>462.84500000000003</v>
+        <v>502.37599999999998</v>
       </c>
       <c r="D23" s="5">
-        <v>212.321</v>
+        <v>253.86</v>
       </c>
       <c r="E23" s="4">
         <v>2.2000000000000002</v>
@@ -1929,16 +1943,16 @@
     </row>
     <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C24" s="5">
-        <v>437.78</v>
+        <v>472.88</v>
       </c>
       <c r="D24" s="5">
-        <v>204.203</v>
+        <v>249.92500000000001</v>
       </c>
       <c r="E24" s="4">
         <v>2.2000000000000002</v>
@@ -1949,16 +1963,16 @@
     </row>
     <row r="25" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C25" s="5">
-        <v>437.78</v>
+        <v>477.488</v>
       </c>
       <c r="D25" s="5">
-        <v>204.203</v>
+        <v>248.185</v>
       </c>
       <c r="E25" s="4">
         <v>2.2000000000000002</v>
@@ -1969,16 +1983,16 @@
     </row>
     <row r="26" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C26" s="5">
-        <v>502.37599999999998</v>
+        <v>511.06</v>
       </c>
       <c r="D26" s="5">
-        <v>253.86</v>
+        <v>244.381</v>
       </c>
       <c r="E26" s="4">
         <v>2.2000000000000002</v>
@@ -1989,39 +2003,36 @@
     </row>
     <row r="27" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
       <c r="C27" s="5">
-        <v>425.517</v>
+        <v>563.47900000000004</v>
       </c>
       <c r="D27" s="5">
-        <v>200.13900000000001</v>
+        <v>243.565</v>
       </c>
       <c r="E27" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G27" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="C28" s="5">
-        <v>556.245</v>
+        <v>479.476</v>
       </c>
       <c r="D28" s="5">
-        <v>300.33699999999999</v>
+        <v>235.89</v>
       </c>
       <c r="E28" s="4">
         <v>2.2000000000000002</v>
@@ -2030,21 +2041,21 @@
         <v>128</v>
       </c>
       <c r="G28" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C29" s="5">
-        <v>477.488</v>
+        <v>502.178</v>
       </c>
       <c r="D29" s="5">
-        <v>248.185</v>
+        <v>234.93600000000001</v>
       </c>
       <c r="E29" s="4">
         <v>2.2000000000000002</v>
@@ -2055,16 +2066,16 @@
     </row>
     <row r="30" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="C30" s="5">
-        <v>459.75299999999999</v>
+        <v>454.88499999999999</v>
       </c>
       <c r="D30" s="5">
-        <v>217.78100000000001</v>
+        <v>234.42699999999999</v>
       </c>
       <c r="E30" s="4">
         <v>2.2000000000000002</v>
@@ -2075,85 +2086,76 @@
     </row>
     <row r="31" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="C31" s="5">
-        <v>547.16499999999996</v>
+        <v>500.24799999999999</v>
       </c>
       <c r="D31" s="5">
-        <v>329.22199999999998</v>
+        <v>234.27600000000001</v>
       </c>
       <c r="E31" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G31" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>82</v>
+        <v>124</v>
       </c>
       <c r="C32" s="5">
-        <v>360.80700000000002</v>
+        <v>497.41699999999997</v>
       </c>
       <c r="D32" s="5">
-        <v>182.56100000000001</v>
+        <v>230.98</v>
       </c>
       <c r="E32" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G32" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
       <c r="C33" s="5">
-        <v>299.41399999999999</v>
+        <v>497.26799999999997</v>
       </c>
       <c r="D33" s="5">
-        <v>169.15799999999999</v>
-      </c>
-      <c r="E33" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" t="s">
-        <v>139</v>
+        <v>230.96</v>
+      </c>
+      <c r="E33">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F33" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="C34" s="5">
-        <v>502.178</v>
+        <v>504.68799999999999</v>
       </c>
       <c r="D34" s="5">
-        <v>234.93600000000001</v>
+        <v>230.749</v>
       </c>
       <c r="E34" s="4">
         <v>2.2000000000000002</v>
@@ -2162,41 +2164,38 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="19" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>152</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="5">
-        <v>519.96400000000006</v>
-      </c>
-      <c r="D35" s="5">
-        <v>304.73</v>
+        <v>135</v>
+      </c>
+      <c r="C35">
+        <v>496.00900000000001</v>
+      </c>
+      <c r="D35">
+        <v>230.708</v>
       </c>
       <c r="E35" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G35" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="C36" s="5">
-        <v>395.529</v>
+        <v>484.94400000000002</v>
       </c>
       <c r="D36" s="5">
-        <v>188.83799999999999</v>
+        <v>230.494</v>
       </c>
       <c r="E36" s="4">
         <v>2.2000000000000002</v>
@@ -2207,16 +2206,16 @@
     </row>
     <row r="37" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="C37" s="5">
-        <v>457.23700000000002</v>
+        <v>491.43599999999998</v>
       </c>
       <c r="D37" s="5">
-        <v>200.39500000000001</v>
+        <v>228.92500000000001</v>
       </c>
       <c r="E37" s="4">
         <v>2.2000000000000002</v>
@@ -2227,122 +2226,125 @@
     </row>
     <row r="38" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C38" s="5">
-        <v>397.24400000000003</v>
+        <v>491.43599999999998</v>
       </c>
       <c r="D38" s="5">
-        <v>201.71600000000001</v>
+        <v>228.92500000000001</v>
       </c>
       <c r="E38" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G38" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="C39" s="5">
-        <v>60.523000000000003</v>
+        <v>491.37799999999999</v>
       </c>
       <c r="D39" s="5">
-        <v>165.733</v>
+        <v>228.90299999999999</v>
       </c>
       <c r="E39" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F39" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" t="s">
-        <v>142</v>
+      <c r="F39" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>163</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C40" s="5">
-        <v>453.13200000000001</v>
+        <v>347.57</v>
       </c>
       <c r="D40" s="5">
-        <v>208.72800000000001</v>
+        <v>226.02</v>
       </c>
       <c r="E40" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G40" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C41" s="5">
-        <v>472.88</v>
+        <v>449.46199999999999</v>
       </c>
       <c r="D41" s="5">
-        <v>249.92500000000001</v>
+        <v>223.166</v>
       </c>
       <c r="E41" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G41" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C42" s="5">
-        <v>468.084</v>
+        <v>547.05899999999997</v>
       </c>
       <c r="D42" s="5">
-        <v>213.631</v>
+        <v>220.21299999999999</v>
       </c>
       <c r="E42" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G42" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C43" s="5">
-        <v>491.43599999999998</v>
+        <v>459.75299999999999</v>
       </c>
       <c r="D43" s="5">
-        <v>228.92500000000001</v>
+        <v>217.78100000000001</v>
       </c>
       <c r="E43" s="4">
         <v>2.2000000000000002</v>
@@ -2353,62 +2355,56 @@
     </row>
     <row r="44" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C44" s="5">
-        <v>429.28300000000002</v>
+        <v>497.25200000000001</v>
       </c>
       <c r="D44" s="5">
-        <v>274.56200000000001</v>
+        <v>215.18199999999999</v>
       </c>
       <c r="E44" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G44" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C45" s="5">
-        <v>657.00800000000004</v>
+        <v>468.084</v>
       </c>
       <c r="D45" s="5">
-        <v>478.9</v>
+        <v>213.631</v>
       </c>
       <c r="E45" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F45" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G45" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>165</v>
+        <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="C46" s="5">
-        <v>491.37799999999999</v>
+        <v>462.84500000000003</v>
       </c>
       <c r="D46" s="5">
-        <v>228.90299999999999</v>
+        <v>212.321</v>
       </c>
       <c r="E46" s="4">
         <v>2.2000000000000002</v>
@@ -2419,39 +2415,36 @@
     </row>
     <row r="47" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="C47" s="5">
-        <v>259.93599999999998</v>
+        <v>451.37400000000002</v>
       </c>
       <c r="D47" s="5">
-        <v>102.52800000000001</v>
+        <v>211.19200000000001</v>
       </c>
       <c r="E47" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G47" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="C48" s="5">
-        <v>311.13099999999997</v>
+        <v>451.37400000000002</v>
       </c>
       <c r="D48" s="5">
-        <v>148.76599999999999</v>
+        <v>211.19200000000001</v>
       </c>
       <c r="E48" s="4">
         <v>2.2000000000000002</v>
@@ -2462,39 +2455,36 @@
     </row>
     <row r="49" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C49" s="5">
-        <v>511.01600000000002</v>
+        <v>453.13200000000001</v>
       </c>
       <c r="D49" s="5">
-        <v>282.154</v>
+        <v>208.72800000000001</v>
       </c>
       <c r="E49" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G49" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="C50" s="5">
-        <v>336.63099999999997</v>
+        <v>434.70100000000002</v>
       </c>
       <c r="D50" s="5">
-        <v>158.99299999999999</v>
+        <v>205.86799999999999</v>
       </c>
       <c r="E50" s="4">
         <v>2.2000000000000002</v>
@@ -2505,62 +2495,56 @@
     </row>
     <row r="51" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C51" s="5">
-        <v>479.476</v>
+        <v>437.78</v>
       </c>
       <c r="D51" s="5">
-        <v>235.89</v>
+        <v>204.203</v>
       </c>
       <c r="E51" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G51" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>166</v>
+        <v>4</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C52" s="5">
-        <v>390.94200000000001</v>
+        <v>437.78</v>
       </c>
       <c r="D52" s="5">
-        <v>186.08699999999999</v>
+        <v>204.203</v>
       </c>
       <c r="E52" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G52" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C53" s="5">
-        <v>484.94400000000002</v>
+        <v>426.83</v>
       </c>
       <c r="D53" s="5">
-        <v>230.494</v>
+        <v>203.99299999999999</v>
       </c>
       <c r="E53" s="4">
         <v>2.2000000000000002</v>
@@ -2571,36 +2555,39 @@
     </row>
     <row r="54" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C54" s="5">
-        <v>491.43599999999998</v>
+        <v>397.24400000000003</v>
       </c>
       <c r="D54" s="5">
-        <v>228.92500000000001</v>
+        <v>201.71600000000001</v>
       </c>
       <c r="E54" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G54" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C55" s="5">
-        <v>395.81400000000002</v>
+        <v>369.94099999999997</v>
       </c>
       <c r="D55" s="5">
-        <v>159.62899999999999</v>
+        <v>201.38499999999999</v>
       </c>
       <c r="E55" s="4">
         <v>2.2000000000000002</v>
@@ -2614,16 +2601,16 @@
     </row>
     <row r="56" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>167</v>
+        <v>15</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C56" s="5">
-        <v>563.47900000000004</v>
+        <v>457.23700000000002</v>
       </c>
       <c r="D56" s="5">
-        <v>243.565</v>
+        <v>200.39500000000001</v>
       </c>
       <c r="E56" s="4">
         <v>2.2000000000000002</v>
@@ -2634,16 +2621,16 @@
     </row>
     <row r="57" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="C57" s="5">
-        <v>369.94099999999997</v>
+        <v>425.517</v>
       </c>
       <c r="D57" s="5">
-        <v>201.38499999999999</v>
+        <v>200.13900000000001</v>
       </c>
       <c r="E57" s="4">
         <v>2.2000000000000002</v>
@@ -2652,21 +2639,21 @@
         <v>128</v>
       </c>
       <c r="G57" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C58" s="5">
-        <v>410.39299999999997</v>
+        <v>395.529</v>
       </c>
       <c r="D58" s="5">
-        <v>164.69300000000001</v>
+        <v>188.83799999999999</v>
       </c>
       <c r="E58" s="4">
         <v>2.2000000000000002</v>
@@ -2677,16 +2664,16 @@
     </row>
     <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>166</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C59" s="5">
-        <v>449.46199999999999</v>
+        <v>390.94200000000001</v>
       </c>
       <c r="D59" s="5">
-        <v>223.166</v>
+        <v>186.08699999999999</v>
       </c>
       <c r="E59" s="4">
         <v>2.2000000000000002</v>
@@ -2695,124 +2682,133 @@
         <v>128</v>
       </c>
       <c r="G59" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>109</v>
+        <v>157</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="C60" s="5">
-        <v>454.88499999999999</v>
+        <v>286.87799999999999</v>
       </c>
       <c r="D60" s="5">
-        <v>234.42699999999999</v>
+        <v>184.35400000000001</v>
       </c>
       <c r="E60" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G60" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="C61" s="5">
-        <v>497.25200000000001</v>
+        <v>360.80700000000002</v>
       </c>
       <c r="D61" s="5">
-        <v>215.18199999999999</v>
+        <v>182.56100000000001</v>
       </c>
       <c r="E61" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G61" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>37</v>
+        <v>160</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="C62" s="5">
-        <v>547.05899999999997</v>
+        <v>407.09100000000001</v>
       </c>
       <c r="D62" s="5">
-        <v>220.21299999999999</v>
+        <v>182.328</v>
       </c>
       <c r="E62" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G62" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
       <c r="C63" s="5">
-        <v>613.40099999999995</v>
+        <v>299.41399999999999</v>
       </c>
       <c r="D63" s="5">
-        <v>457.71</v>
+        <v>169.15799999999999</v>
       </c>
       <c r="E63" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G63" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C64" s="5">
-        <v>547.33600000000001</v>
+        <v>60.523000000000003</v>
       </c>
       <c r="D64" s="5">
-        <v>267.74400000000003</v>
+        <v>165.733</v>
       </c>
       <c r="E64" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>128</v>
+      <c r="F64" t="s">
+        <v>129</v>
+      </c>
+      <c r="G64" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C65" s="5">
-        <v>434.70100000000002</v>
+        <v>410.39299999999997</v>
       </c>
       <c r="D65" s="5">
-        <v>205.86799999999999</v>
+        <v>164.69300000000001</v>
       </c>
       <c r="E65" s="4">
         <v>2.2000000000000002</v>
@@ -2823,16 +2819,16 @@
     </row>
     <row r="66" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C66" s="5">
-        <v>576.09500000000003</v>
+        <v>395.81400000000002</v>
       </c>
       <c r="D66" s="5">
-        <v>257.839</v>
+        <v>159.62899999999999</v>
       </c>
       <c r="E66" s="4">
         <v>2.2000000000000002</v>
@@ -2841,21 +2837,21 @@
         <v>128</v>
       </c>
       <c r="G66" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>27</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="C67" s="5">
-        <v>426.83</v>
+        <v>336.63099999999997</v>
       </c>
       <c r="D67" s="5">
-        <v>203.99299999999999</v>
+        <v>158.99299999999999</v>
       </c>
       <c r="E67" s="4">
         <v>2.2000000000000002</v>
@@ -2866,16 +2862,16 @@
     </row>
     <row r="68" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="C68" s="5">
-        <v>511.06</v>
+        <v>311.13099999999997</v>
       </c>
       <c r="D68" s="5">
-        <v>244.381</v>
+        <v>148.76599999999999</v>
       </c>
       <c r="E68" s="4">
         <v>2.2000000000000002</v>
@@ -2886,56 +2882,62 @@
     </row>
     <row r="69" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="C69" s="5">
-        <v>579.18700000000001</v>
+        <v>257.899</v>
       </c>
       <c r="D69" s="5">
-        <v>303.61900000000003</v>
+        <v>135.018</v>
       </c>
       <c r="E69" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G69" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>118</v>
+        <v>158</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="C70" s="5">
-        <v>451.37400000000002</v>
+        <v>232.20400000000001</v>
       </c>
       <c r="D70" s="5">
-        <v>211.19200000000001</v>
+        <v>120.45099999999999</v>
       </c>
       <c r="E70" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F70" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G70" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>44</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>119</v>
+        <v>155</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="C71" s="5">
-        <v>504.68799999999999</v>
+        <v>253.49700000000001</v>
       </c>
       <c r="D71" s="5">
-        <v>230.749</v>
+        <v>115.92100000000001</v>
       </c>
       <c r="E71" s="4">
         <v>2.2000000000000002</v>
@@ -2946,163 +2948,163 @@
     </row>
     <row r="72" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
       <c r="C72" s="5">
-        <v>500.24799999999999</v>
+        <v>259.93599999999998</v>
       </c>
       <c r="D72" s="5">
-        <v>234.27600000000001</v>
+        <v>102.52800000000001</v>
       </c>
       <c r="E72" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>128</v>
+      </c>
+      <c r="G72" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="C73" s="5">
-        <v>448.435</v>
+        <v>260.495</v>
       </c>
       <c r="D73" s="5">
-        <v>263.34899999999999</v>
+        <v>95.259</v>
       </c>
       <c r="E73" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="G73" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>47</v>
+        <v>173</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="C74" s="5">
-        <v>629.94399999999996</v>
+        <v>256.959</v>
       </c>
       <c r="D74" s="5">
-        <v>344.88299999999998</v>
-      </c>
-      <c r="E74" s="4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G74" t="s">
-        <v>133</v>
+        <v>69.838999999999999</v>
+      </c>
+      <c r="E74">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F74" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="C75" s="5">
-        <v>497.41699999999997</v>
+        <v>171.90299999999999</v>
       </c>
       <c r="D75" s="5">
-        <v>230.98</v>
+        <v>51.412999999999997</v>
       </c>
       <c r="E75" s="4">
         <v>2.2000000000000002</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="G75" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:B74">
-    <sortCondition ref="A1"/>
+  <sortState ref="A2:G76">
+    <sortCondition descending="1" ref="D1"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B13" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B17" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B21" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B22" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B23" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B24" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B25" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B26" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B27" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="B29" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="B30" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="B31" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="B32" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="B33" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B34" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="B35" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="B36" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B37" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="B38" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="B39" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="B40" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="B41" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="B42" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B43" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="B44" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B45" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B47" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="B48" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="B49" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="B50" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="B51" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="B52" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="B53" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="B54" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="B55" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="B56" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="B57" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="B58" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="B59" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="B60" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="B61" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="B62" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="B64" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="B65" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="B66" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="B67" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="B68" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="B69" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="B70" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="B71" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="B72" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="B73" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="B74" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="B46" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="B75" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="B5" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="B20" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="B28" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="B63" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="B3" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="B2" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="B47" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B62" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B75" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B73" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B69" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B46" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B51" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B52" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B57" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B25" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B43" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B10" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B61" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B63" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B12" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B58" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B56" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B54" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B64" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B49" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B24" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B45" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B37" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B19" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B3" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B72" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B68" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B16" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B67" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B28" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B59" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B36" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B38" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B66" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B27" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B55" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B65" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B41" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="B30" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="B44" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="B42" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="B20" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="B50" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="B22" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="B53" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="B26" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="B13" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="B48" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="B34" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="B31" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="B21" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="B8" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="B39" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="B32" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="B7" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="B35" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="B14" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="B4" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="B33" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="B74" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>